<commit_message>
Úprava SWOT - přidány strategie
</commit_message>
<xml_diff>
--- a/Diagrams/SWOT.xlsx
+++ b/Diagrams/SWOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/79ce744038a9155a/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaMA\Documents\GitHub\swinzrepository\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{ED55AC6F-89BD-46D8-9F9D-DC8F1DD0F9B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{78942AA6-3220-469A-A369-F59E7011C150}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4377C3A7-8FBA-41BA-841D-3A279E5A9D97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SWOT Comparison" sheetId="2" r:id="rId1"/>
@@ -42,27 +42,6 @@
     <t>Hrozby</t>
   </si>
   <si>
-    <t>Freeware, podpora 24/7</t>
-  </si>
-  <si>
-    <t>Vše digitálně a přehledně</t>
-  </si>
-  <si>
-    <t>Lukrativní pracovní místa</t>
-  </si>
-  <si>
-    <t>Nedostatek zaměstnanců</t>
-  </si>
-  <si>
-    <t>Intuitivnost aplikace</t>
-  </si>
-  <si>
-    <t>Architektura aplikace</t>
-  </si>
-  <si>
-    <t>Úspěšná konkurence</t>
-  </si>
-  <si>
     <t>CSA/A (Car Servis Administration / Application) SWOT</t>
   </si>
   <si>
@@ -72,16 +51,37 @@
     <t>Možnost chyby lidského faktoru -&gt; Školení zaměstnanců</t>
   </si>
   <si>
-    <t>Ztráta dat -&gt; Záloha dat</t>
-  </si>
-  <si>
     <t>Zastaralost aplikace -&gt; Použít nové programovací technologie</t>
   </si>
   <si>
     <t>Výpadek systému (internetu, či elektřiny) -&gt; Záložní generátor (baterie), offline režim</t>
   </si>
   <si>
-    <t>Nutnost správného hardwaru -&gt; Investice do hardwaru</t>
+    <t>Úspěšná konkurence -&gt; Každý měsíc kontrolovat stav konkurence, analyzovat jejich strategii a úspěšnost</t>
+  </si>
+  <si>
+    <t>Ztráta dat -&gt;  Denní záloha, která bude uložena po dobu 60 dní, trvalé měsíční zálohy</t>
+  </si>
+  <si>
+    <t>Lukrativní pracovní místa -&gt; Home Office, týmové akce, zajímavý záznam do životopisu</t>
+  </si>
+  <si>
+    <t>Intuitivnost aplikace -&gt; Jednoduchý formulář, který uživateli nedovolí dělat chyby</t>
+  </si>
+  <si>
+    <t>Vše digitálně a přehledně -&gt; Přehledný výpis z databáze do tabulky</t>
+  </si>
+  <si>
+    <t>Nedostatek zaměstnanců -&gt; Vytvoření likrativních pracovních míst, dobrá pověst firmy</t>
+  </si>
+  <si>
+    <t>Freeware, podpora 24/7 -&gt; Neomezená podpora je zpoplatněná, díky tomu může být aplikace freeware</t>
+  </si>
+  <si>
+    <t>Nutnost správného hardwaru -&gt; Investice do hardwaru, nenáročnost aplikace</t>
+  </si>
+  <si>
+    <t>Architektura aplikace -&gt; Aplikace je snadno upravitelná a přehledně zdokumentovaná</t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -179,21 +179,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color theme="1" tint="0.34998626667073579"/>
       </top>
       <bottom style="thin">
@@ -249,19 +234,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color theme="1" tint="0.34998626667073579"/>
@@ -353,23 +325,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.24994659260841701"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -378,10 +339,25 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="1" tint="0.34998626667073579"/>
       </top>
       <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -393,9 +369,24 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -405,54 +396,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -474,75 +418,72 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -892,8 +833,8 @@
   </sheetPr>
   <dimension ref="B1:C27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -908,10 +849,10 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="2:3" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="7"/>
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="2:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -922,73 +863,73 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="2:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+    </row>
+    <row r="12" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="13"/>
-    </row>
-    <row r="7" spans="2:3" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="21"/>
-      <c r="C13" s="22" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>